<commit_message>
adds pictures and updates files
</commit_message>
<xml_diff>
--- a/Notebooks/top_20_city_pairs.xlsx
+++ b/Notebooks/top_20_city_pairs.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fakhi\Desktop\db1b stuff\part4_DB1BMarket_2025_2\Notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FB932A-C0EB-4F62-9460-2334D8AF60B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC706E18-C1FC-4050-8B51-A149F22E00E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB08ED52-A972-4F54-A938-3744B46997B7}"/>
   </bookViews>
   <sheets>
     <sheet name="top_20_city_pairs" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">top_20_city_pairs!$K$3:$L$12</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">top_20_city_pairs!$M$2</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">top_20_city_pairs!$M$3:$M$12</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>City-Pair</t>
   </si>
@@ -43,13 +51,7 @@
     <t>EWR-SFO</t>
   </si>
   <si>
-    <t>2589.7678715670436</t>
-  </si>
-  <si>
     <t>LGA-ORD</t>
-  </si>
-  <si>
-    <t>733.1437651897551</t>
   </si>
   <si>
     <t>EWR-LAX</t>
@@ -58,73 +60,37 @@
     <t>ORD-SFO</t>
   </si>
   <si>
-    <t>1879.070885256514</t>
-  </si>
-  <si>
     <t>EWR-MCO</t>
-  </si>
-  <si>
-    <t>946.7147912243454</t>
   </si>
   <si>
     <t>EWR-ORD</t>
   </si>
   <si>
-    <t>729.9326186830016</t>
-  </si>
-  <si>
     <t>IAD-LAX</t>
-  </si>
-  <si>
-    <t>2301.1779975278123</t>
   </si>
   <si>
     <t>DEN-ORD</t>
   </si>
   <si>
-    <t>920.8155697445973</t>
-  </si>
-  <si>
     <t>LAX-ORD</t>
-  </si>
-  <si>
-    <t>1760.986095537116</t>
   </si>
   <si>
     <t>EWR-LAS</t>
   </si>
   <si>
-    <t>2243.8799188640974</t>
-  </si>
-  <si>
     <t>EWR-PBI</t>
-  </si>
-  <si>
-    <t>1024.5107913669065</t>
   </si>
   <si>
     <t>EWR-FLL</t>
   </si>
   <si>
-    <t>1069.6843998971988</t>
-  </si>
-  <si>
     <t>LAX-SFO</t>
-  </si>
-  <si>
-    <t>340.6813271604938</t>
   </si>
   <si>
     <t>IAH-LGA</t>
   </si>
   <si>
-    <t>1419.924578527063</t>
-  </si>
-  <si>
     <t>BOS-ORD</t>
-  </si>
-  <si>
-    <t>869.6672108843537</t>
   </si>
   <si>
     <t>DCA-ORD</t>
@@ -133,35 +99,36 @@
     <t>DEN-SFO</t>
   </si>
   <si>
-    <t>985.7296340023613</t>
-  </si>
-  <si>
     <t>IAD-SFO</t>
-  </si>
-  <si>
-    <t>2441.6555938037864</t>
   </si>
   <si>
     <t>IAH-ORD</t>
   </si>
   <si>
-    <t>953.1888780009799</t>
-  </si>
-  <si>
     <t>SAN-SFO</t>
   </si>
   <si>
-    <t>446.9986454453099</t>
+    <t xml:space="preserve"> Passengers_Estimated</t>
   </si>
   <si>
-    <t>TotalEstimatedPassengers</t>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>2025 Q1</t>
+  </si>
+  <si>
+    <t>2025 Q2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +259,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -594,7 +567,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -637,12 +610,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -670,6 +646,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -688,6 +665,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF8A206"/>
+      <color rgb="FFFDAD03"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -700,6 +683,404 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1254985035579077"/>
+          <c:y val="0.13645408013343444"/>
+          <c:w val="0.83182684489550929"/>
+          <c:h val="0.78041224913575058"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]top_20_city_pairs!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Passengers_Estimated </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="12700"/>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]top_20_city_pairs!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v> EWR-SFO </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> EWR-MCO </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> EWR-LAX </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> EWR-PBI </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> EWR-FLL </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>EWR-MIA</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>EWR-ORD</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MCO-ORD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ORD-SFO</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>EWR-TPA</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>EWR-LAS</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LGA-ORD</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>EWR-RSW</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>EWR-IAH</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>DEN-ORD</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>LAX-SFO</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>LAX-ORD</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>DEN-EWR</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>DEN-IAH</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>ORD-RSW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]top_20_city_pairs!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>255900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253650</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>219240</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191860</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>179170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>164360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>161060</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>158970</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>156200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>152030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>139840</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131150</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>127290</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>123870</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>122430</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>120610</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>115710</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>114680</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>113450</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F205-45A5-A89C-7E5B5111A247}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="60"/>
+        <c:axId val="1499308543"/>
+        <c:axId val="1499306623"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1499308543"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="30" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1499306623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1499306623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1499308543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr algn="ctr">
+        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter>
+      <c:oddFooter>Prepared by Fakhir &amp;D&amp;RPage &amp;P</c:oddFooter>
+    </c:headerFooter>
+    <c:pageMargins b="0.74803149606299213" l="0.70866141732283472" r="0.70866141732283472" t="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+  <c:userShapes r:id="rId4"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -802,11 +1183,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>top_20_city_pairs!$I$4</c:f>
+              <c:f>top_20_city_pairs!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TotalEstimatedPassengers</c:v>
+                  <c:v> Passengers_Estimated</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -886,7 +1267,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>top_20_city_pairs!$C$5:$C$24</c:f>
+              <c:f>top_20_city_pairs!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -954,9 +1335,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>top_20_city_pairs!$I$5:$I$24</c:f>
+              <c:f>top_20_city_pairs!$G$2:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>318310</c:v>
@@ -1042,7 +1423,7 @@
       <c:catAx>
         <c:axId val="1296244479"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1096,8 +1477,8 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1112,92 +1493,10 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-CA"/>
-                  <a:t>Passengers</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1296244479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1247,6 +1546,174 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>United Airlines Top 5 City-Pairs (Source: DB1B)</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400" b="0" i="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" b="1">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="AGaramond RegularSC" panose="02020500000000000000" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>United Airlines Top 5 City-Pairs (Source: DB1B)</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="treemap" uniqueId="{57547F73-F568-4E7A-AF51-44977A5C7375}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:v> Passengers_Estimated</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataPt idx="6">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataLabels pos="inEnd">
+            <cx:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <cx:txPr>
+              <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="1050" b="0" i="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:solidFill>
+                      <a:srgbClr val="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-CA" sz="1050">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator>
+</cx:separator>
+            <cx:dataLabel idx="0">
+              <cx:numFmt formatCode="#,##0" sourceLinked="0"/>
+              <cx:txPr>
+                <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr" rtl="0">
+                    <a:defRPr sz="1100"/>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="window" lastClr="FFFFFF"/>
+                      </a:solidFill>
+                      <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <a:t>2025 Q1</a:t>
+                  </a:r>
+                </a:p>
+              </cx:txPr>
+              <cx:visibility seriesName="0" categoryName="1" value="1"/>
+              <cx:separator>
+</cx:separator>
+            </cx:dataLabel>
+            <cx:dataLabel idx="6">
+              <cx:numFmt formatCode="#,##0" sourceLinked="0"/>
+              <cx:txPr>
+                <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr" rtl="0">
+                    <a:defRPr sz="1100" b="1">
+                      <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                      <a:cs typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="window" lastClr="FFFFFF"/>
+                      </a:solidFill>
+                      <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <a:t>2025 Q2</a:t>
+                  </a:r>
+                </a:p>
+              </cx:txPr>
+              <cx:visibility seriesName="0" categoryName="1" value="1"/>
+              <cx:separator>
+</cx:separator>
+            </cx:dataLabel>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:parentLabelLayout val="banner"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </a:solidFill>
+  </cx:spPr>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1287,7 +1754,609 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1792,20 +2861,641 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>906780</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>11419</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6E54C1-D405-F6C9-6C78-FDD7BD6E37B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9387840" y="2682240"/>
+              <a:ext cx="6568440" cy="3733800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>173113</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>166677</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>150771</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FF5EC31-7FDC-4C4B-BA54-F68393DC24B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>102858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1203960</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>175259</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1826,13 +3516,450 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.01071</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96499</cdr:x>
+      <cdr:y>0.12755</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A5DFAF9-A705-5D7B-EE13-12D434F73215}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="50581"/>
+          <a:ext cx="7560442" cy="551793"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1800" b="0" i="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="AGaramond RegularSC" panose="02020500000000000000" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>United Airlines Q1 2025: Top 10 Domestic City‑Pairs by Passenger Volume</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA">
+            <a:effectLst/>
+            <a:latin typeface="AGaramond RegularSC" panose="02020500000000000000" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Passenger volumes are estimated from DB1B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1200">
+            <a:effectLst/>
+            <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.03104</cdr:x>
+      <cdr:y>0.95242</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19298</cdr:x>
+      <cdr:y>0.99775</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D1D2D92-B085-C896-58A6-396C36062EF4}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="277585" y="4764568"/>
+          <a:ext cx="1448175" cy="226777"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-CA" sz="1100" kern="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.03431</cdr:x>
+      <cdr:y>0.93577</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19063</cdr:x>
+      <cdr:y>0.98829</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CEF6CBE-7520-39E8-E6B4-B3F27525FC37}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="306863" y="4681290"/>
+          <a:ext cx="1397876" cy="262759"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-CA" sz="1100" kern="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02419</cdr:x>
+      <cdr:y>0.93157</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.20733</cdr:x>
+      <cdr:y>0.98146</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC00CCC7-6938-9EEE-66B0-D40E23908FF1}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="217524" y="4660270"/>
+          <a:ext cx="1646756" cy="249600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-CA" sz="1000" kern="1200">
+              <a:latin typeface="Adobe Garamond Pro" panose="02020502060506020403" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Source: transtats.bts.gov</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="top_20_city_pairs"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="G1" t="str">
+            <v>Passengers_Estimated</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>EWR-SFO</v>
+          </cell>
+          <cell r="G2">
+            <v>255900</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>EWR-MCO</v>
+          </cell>
+          <cell r="G3">
+            <v>253650</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>EWR-LAX</v>
+          </cell>
+          <cell r="G4">
+            <v>219240</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>EWR-PBI</v>
+          </cell>
+          <cell r="G5">
+            <v>210300</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>EWR-FLL</v>
+          </cell>
+          <cell r="G6">
+            <v>191860</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>EWR-MIA</v>
+          </cell>
+          <cell r="G7">
+            <v>179170</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>EWR-ORD</v>
+          </cell>
+          <cell r="G8">
+            <v>164360</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>MCO-ORD</v>
+          </cell>
+          <cell r="G9">
+            <v>161060</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>ORD-SFO</v>
+          </cell>
+          <cell r="G10">
+            <v>158970</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>EWR-TPA</v>
+          </cell>
+          <cell r="G11">
+            <v>156200</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>EWR-LAS</v>
+          </cell>
+          <cell r="G12">
+            <v>152030</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>LGA-ORD</v>
+          </cell>
+          <cell r="G13">
+            <v>139840</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>EWR-RSW</v>
+          </cell>
+          <cell r="G14">
+            <v>131150</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>EWR-IAH</v>
+          </cell>
+          <cell r="G15">
+            <v>127290</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>DEN-ORD</v>
+          </cell>
+          <cell r="G16">
+            <v>123870</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>LAX-SFO</v>
+          </cell>
+          <cell r="G17">
+            <v>122430</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>LAX-ORD</v>
+          </cell>
+          <cell r="G18">
+            <v>120610</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>DEN-EWR</v>
+          </cell>
+          <cell r="G19">
+            <v>115710</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>DEN-IAH</v>
+          </cell>
+          <cell r="G20">
+            <v>114680</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>ORD-RSW</v>
+          </cell>
+          <cell r="G21">
+            <v>113450</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2150,509 +4277,898 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="0E2841"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E8E8E8"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="156082"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="E97132"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="196B24"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="0F9ED5"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="A02B93"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="4EA72E"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="467886"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="96607D"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9789BAE-39F2-4AE3-829B-0627D117B93D}">
-  <dimension ref="C4:I24"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
-        <v>44</v>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="B2" s="1">
         <v>31831</v>
       </c>
-      <c r="E5">
+      <c r="C2" s="1">
         <v>780.41223000000002</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="D2" s="2">
+        <v>2589.7678715670399</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2589.7678715670399</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2565</v>
+      </c>
+      <c r="G2" s="3">
+        <v>318310</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="B3" s="1">
+        <v>28599</v>
+      </c>
+      <c r="C3" s="1">
+        <v>317.67676</v>
+      </c>
+      <c r="D3" s="2">
+        <v>733.14376518975496</v>
+      </c>
+      <c r="E3" s="2">
+        <v>733.14376518975496</v>
+      </c>
+      <c r="F3" s="1">
+        <v>733</v>
+      </c>
+      <c r="G3" s="3">
+        <v>285990</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <v>255900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>27189</v>
+      </c>
+      <c r="C4" s="1">
+        <v>681.54693999999995</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2468.4769415853498</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2468.4769415853498</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2454</v>
+      </c>
+      <c r="G4" s="3">
+        <v>271890</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>253650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23027</v>
+      </c>
+      <c r="C5" s="1">
+        <v>433.78226000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1879.0708852565101</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1879.0708852565101</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1846</v>
+      </c>
+      <c r="G5" s="3">
+        <v>230270</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="1">
+        <v>219240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>22009</v>
+      </c>
+      <c r="C6" s="1">
+        <v>316.27386000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>946.71479122434505</v>
+      </c>
+      <c r="E6" s="2">
+        <v>946.71479122434505</v>
+      </c>
+      <c r="F6" s="1">
+        <v>937</v>
+      </c>
+      <c r="G6" s="3">
+        <v>220090</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1">
+        <v>210300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>18637</v>
+      </c>
+      <c r="C7" s="1">
+        <v>329.31848000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>729.93261868300101</v>
+      </c>
+      <c r="E7" s="2">
+        <v>729.93261868300101</v>
+      </c>
+      <c r="F7" s="1">
+        <v>719</v>
+      </c>
+      <c r="G7" s="3">
+        <v>186370</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="1">
+        <v>191860</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>16390</v>
+      </c>
+      <c r="C8" s="1">
+        <v>439.60367000000002</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2301.17799752781</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2301.17799752781</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2288</v>
+      </c>
+      <c r="G8" s="3">
+        <v>163900</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>318310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>15631</v>
+      </c>
+      <c r="C9" s="1">
+        <v>294.16300000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>920.81556974459704</v>
+      </c>
+      <c r="E9" s="2">
+        <v>920.81556974459704</v>
+      </c>
+      <c r="F9" s="1">
+        <v>888</v>
+      </c>
+      <c r="G9" s="3">
+        <v>156310</v>
+      </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" t="s">
         <v>7</v>
       </c>
-      <c r="H5">
-        <v>2565</v>
-      </c>
-      <c r="I5">
-        <v>318310</v>
+      <c r="M9" s="1">
+        <v>285990</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>15588</v>
+      </c>
+      <c r="C10" s="1">
+        <v>386.23836999999997</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1760.98609553711</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1760.98609553711</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1744</v>
+      </c>
+      <c r="G10" s="3">
+        <v>155880</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
-        <v>28599</v>
-      </c>
-      <c r="E6">
-        <v>317.67676</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="M10" s="1">
+        <v>271890</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>15103</v>
+      </c>
+      <c r="C11" s="1">
+        <v>487.83535999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2243.8799188640901</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2243.8799188640901</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2227</v>
+      </c>
+      <c r="G11" s="3">
+        <v>151030</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>733</v>
-      </c>
-      <c r="I6">
-        <v>285990</v>
+      <c r="M11" s="1">
+        <v>230270</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>14938</v>
+      </c>
+      <c r="C12" s="1">
+        <v>350.74340000000001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1024.5107913669001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1024.5107913669001</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1023</v>
+      </c>
+      <c r="G12" s="3">
+        <v>149380</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="D7">
-        <v>27189</v>
-      </c>
-      <c r="E7">
-        <v>681.54693999999995</v>
-      </c>
-      <c r="F7">
-        <v>2468.4769415853498</v>
-      </c>
-      <c r="G7">
-        <v>2468.4769415853498</v>
-      </c>
-      <c r="H7">
-        <v>2454</v>
-      </c>
-      <c r="I7">
-        <v>271890</v>
+      <c r="M12" s="1">
+        <v>220090</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>23027</v>
-      </c>
-      <c r="E8">
-        <v>433.78226000000001</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>1846</v>
-      </c>
-      <c r="I8">
-        <v>230270</v>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>14544</v>
+      </c>
+      <c r="C13" s="1">
+        <v>320.69693000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1069.6843998971899</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1069.6843998971899</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1065</v>
+      </c>
+      <c r="G13" s="3">
+        <v>145440</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>22009</v>
-      </c>
-      <c r="E9">
-        <v>316.27386000000001</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9">
-        <v>937</v>
-      </c>
-      <c r="I9">
-        <v>220090</v>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>14333</v>
+      </c>
+      <c r="C14" s="1">
+        <v>212.52248</v>
+      </c>
+      <c r="D14" s="2">
+        <v>340.68132716049303</v>
+      </c>
+      <c r="E14" s="2">
+        <v>340.68132716049303</v>
+      </c>
+      <c r="F14" s="1">
+        <v>337</v>
+      </c>
+      <c r="G14" s="3">
+        <v>143330</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>18637</v>
-      </c>
-      <c r="E10">
-        <v>329.31848000000002</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10">
-        <v>719</v>
-      </c>
-      <c r="I10">
-        <v>186370</v>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14206</v>
+      </c>
+      <c r="C15" s="1">
+        <v>373.65607</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1419.92457852706</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1419.92457852706</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1416</v>
+      </c>
+      <c r="G15" s="3">
+        <v>142060</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11">
-        <v>16390</v>
-      </c>
-      <c r="E11">
-        <v>439.60367000000002</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11">
-        <v>2288</v>
-      </c>
-      <c r="I11">
-        <v>163900</v>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
+        <v>14114</v>
+      </c>
+      <c r="C16" s="1">
+        <v>258.33566000000002</v>
+      </c>
+      <c r="D16" s="2">
+        <v>869.66721088435304</v>
+      </c>
+      <c r="E16" s="2">
+        <v>869.66721088435304</v>
+      </c>
+      <c r="F16" s="1">
+        <v>867</v>
+      </c>
+      <c r="G16" s="3">
+        <v>141140</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12">
-        <v>15631</v>
-      </c>
-      <c r="E12">
-        <v>294.16300000000001</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12">
-        <v>888</v>
-      </c>
-      <c r="I12">
-        <v>156310</v>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>13908</v>
+      </c>
+      <c r="C17" s="1">
+        <v>262.36047000000002</v>
+      </c>
+      <c r="D17" s="1">
+        <v>612</v>
+      </c>
+      <c r="E17" s="1">
+        <v>612</v>
+      </c>
+      <c r="F17" s="1">
+        <v>612</v>
+      </c>
+      <c r="G17" s="3">
+        <v>139080</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13">
-        <v>15588</v>
-      </c>
-      <c r="E13">
-        <v>386.23836999999997</v>
-      </c>
-      <c r="F13" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13">
-        <v>1744</v>
-      </c>
-      <c r="I13">
-        <v>155880</v>
+      <c r="B18" s="1">
+        <v>13776</v>
+      </c>
+      <c r="C18" s="1">
+        <v>301.23383000000001</v>
+      </c>
+      <c r="D18" s="2">
+        <v>985.72963400236097</v>
+      </c>
+      <c r="E18" s="2">
+        <v>985.72963400236097</v>
+      </c>
+      <c r="F18" s="1">
+        <v>967</v>
+      </c>
+      <c r="G18" s="3">
+        <v>137760</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="D14">
-        <v>15103</v>
-      </c>
-      <c r="E14">
-        <v>487.83535999999998</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="B19" s="1">
+        <v>13730</v>
+      </c>
+      <c r="C19" s="1">
+        <v>530.45699999999999</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2441.65559380378</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2441.65559380378</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2419</v>
+      </c>
+      <c r="G19" s="3">
+        <v>137300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14">
-        <v>2227</v>
-      </c>
-      <c r="I14">
-        <v>151030</v>
+      <c r="B20" s="1">
+        <v>13541</v>
+      </c>
+      <c r="C20" s="1">
+        <v>305.26233000000002</v>
+      </c>
+      <c r="D20" s="2">
+        <v>953.188878000979</v>
+      </c>
+      <c r="E20" s="2">
+        <v>953.188878000979</v>
+      </c>
+      <c r="F20" s="1">
+        <v>925</v>
+      </c>
+      <c r="G20" s="3">
+        <v>135410</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="D15">
-        <v>14938</v>
-      </c>
-      <c r="E15">
-        <v>350.74340000000001</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15">
-        <v>1023</v>
-      </c>
-      <c r="I15">
-        <v>149380</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16">
-        <v>14544</v>
-      </c>
-      <c r="E16">
-        <v>320.69693000000001</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16">
-        <v>1065</v>
-      </c>
-      <c r="I16">
-        <v>145440</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17">
-        <v>14333</v>
-      </c>
-      <c r="E17">
-        <v>212.52248</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17">
-        <v>337</v>
-      </c>
-      <c r="I17">
-        <v>143330</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18">
-        <v>14206</v>
-      </c>
-      <c r="E18">
-        <v>373.65607</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18">
-        <v>1416</v>
-      </c>
-      <c r="I18">
-        <v>142060</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19">
-        <v>14114</v>
-      </c>
-      <c r="E19">
-        <v>258.33566000000002</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19">
-        <v>867</v>
-      </c>
-      <c r="I19">
-        <v>141140</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20">
-        <v>13908</v>
-      </c>
-      <c r="E20">
-        <v>262.36047000000002</v>
-      </c>
-      <c r="F20">
-        <v>612</v>
-      </c>
-      <c r="G20">
-        <v>612</v>
-      </c>
-      <c r="H20">
-        <v>612</v>
-      </c>
-      <c r="I20">
-        <v>139080</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21">
-        <v>13776</v>
-      </c>
-      <c r="E21">
-        <v>301.23383000000001</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21">
-        <v>967</v>
-      </c>
-      <c r="I21">
-        <v>137760</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22">
-        <v>13730</v>
-      </c>
-      <c r="E22">
-        <v>530.45699999999999</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22">
-        <v>2419</v>
-      </c>
-      <c r="I22">
-        <v>137300</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23">
-        <v>13541</v>
-      </c>
-      <c r="E23">
-        <v>305.26233000000002</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H23">
-        <v>925</v>
-      </c>
-      <c r="I23">
-        <v>135410</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24">
+      <c r="B21" s="1">
         <v>13476</v>
       </c>
-      <c r="E24">
+      <c r="C21" s="1">
         <v>194.87923000000001</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24">
+      <c r="D21" s="2">
+        <v>446.99864544530902</v>
+      </c>
+      <c r="E21" s="2">
+        <v>446.99864544530902</v>
+      </c>
+      <c r="F21" s="1">
         <v>447</v>
       </c>
-      <c r="I24">
+      <c r="G21" s="3">
         <v>134760</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>